<commit_message>
NBS filling input and save button done
</commit_message>
<xml_diff>
--- a/NBSForm.xlsx
+++ b/NBSForm.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\winnie\Desktop\code playground\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Han Ming\Documents\Han Ming\python learning\IFAST-automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A3B7D9-2900-4D7E-9A9D-59A51489A4BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3224BCD6-390A-4AF5-BAD9-833ADA232892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8A7072F4-A22C-4164-AF93-3B95E41BB2A7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8A7072F4-A22C-4164-AF93-3B95E41BB2A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -62,9 +62,6 @@
     <t>Amount Invested</t>
   </si>
   <si>
-    <t xml:space="preserve">Product </t>
-  </si>
-  <si>
     <t>FAF's</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>2000 - test</t>
+  </si>
+  <si>
+    <t>Product</t>
   </si>
 </sst>
 </file>
@@ -482,24 +482,24 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
     <col min="8" max="8" width="9" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" customWidth="1"/>
     <col min="10" max="10" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -510,7 +510,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -522,21 +522,21 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
@@ -545,10 +545,10 @@
         <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="G2" s="2">
         <v>0</v>
@@ -560,20 +560,23 @@
         <v>0</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
         <v>16</v>
       </c>
+      <c r="M4" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="M4" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M5" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="M5" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nbs changed, check for f2f value
</commit_message>
<xml_diff>
--- a/NBSForm.xlsx
+++ b/NBSForm.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Han Ming\Documents\Han Ming\python learning\IFAST-automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\winnie\Desktop\code playground\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3224BCD6-390A-4AF5-BAD9-833ADA232892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7811DB-9F9E-4366-9396-B990DBC38099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8A7072F4-A22C-4164-AF93-3B95E41BB2A7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8A7072F4-A22C-4164-AF93-3B95E41BB2A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Acc No.</t>
   </si>
@@ -65,37 +65,31 @@
     <t>FAF's</t>
   </si>
   <si>
-    <t>FAF Percentage</t>
-  </si>
-  <si>
-    <t>FAF Frequency</t>
-  </si>
-  <si>
     <t>Top Up</t>
   </si>
   <si>
-    <t>Singh, Deepak</t>
-  </si>
-  <si>
     <t>1- Yes</t>
   </si>
   <si>
     <t>0 - No</t>
   </si>
   <si>
-    <t>Annually</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>P0459370</t>
   </si>
   <si>
-    <t>2000 - test</t>
-  </si>
-  <si>
     <t>Product</t>
+  </si>
+  <si>
+    <t>Investment Currency</t>
+  </si>
+  <si>
+    <t>Purdy, Tim</t>
+  </si>
+  <si>
+    <t>USD</t>
   </si>
 </sst>
 </file>
@@ -479,27 +473,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F79661F3-7C3F-4E3B-B974-740FF234562B}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="9" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" customWidth="1"/>
-    <col min="10" max="10" width="18" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="3" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" customWidth="1"/>
+    <col min="11" max="11" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -507,51 +501,48 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2">
+        <v>5011</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="2">
-        <v>0</v>
+      <c r="G2" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="H2" s="2">
         <v>0</v>
@@ -559,24 +550,21 @@
       <c r="I2" s="2">
         <v>0</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="F3" s="2"/>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="M4" t="s">
-        <v>13</v>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="M5" t="s">
-        <v>14</v>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
processing, partial To Payout, click all checkboxes in expected in completed
</commit_message>
<xml_diff>
--- a/NBSForm.xlsx
+++ b/NBSForm.xlsx
@@ -5,22 +5,23 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Han Ming\Documents\Han Ming\python learning\IFAST-automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\winnie\Desktop\code playground\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD94946B-FF2D-4E41-9BCD-117BDF27DBBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D30BCC79-FB01-4480-9B66-54E41105AC1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="tested" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t>Acc No.</t>
   </si>
@@ -77,6 +78,24 @@
   </si>
   <si>
     <t>Date Issued</t>
+  </si>
+  <si>
+    <t>P0333284</t>
+  </si>
+  <si>
+    <t>SGD</t>
+  </si>
+  <si>
+    <t>Singh, Deepak</t>
+  </si>
+  <si>
+    <t>P0519914</t>
+  </si>
+  <si>
+    <t>AUD</t>
+  </si>
+  <si>
+    <t>Brown, Jarrad</t>
   </si>
 </sst>
 </file>
@@ -140,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -157,6 +176,15 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -467,26 +495,26 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -518,15 +546,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="4">
-        <v>5011</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
+    <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="10">
+        <v>13</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>11</v>
@@ -537,31 +565,26 @@
       <c r="F2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="4">
+      <c r="G2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="10">
         <v>0</v>
       </c>
-      <c r="I2" s="4">
-        <v>0</v>
+      <c r="I2" s="10">
+        <v>1</v>
       </c>
       <c r="J2" s="7">
-        <v>45467</v>
+        <v>45337</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
+    <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N5" t="s">
         <v>17</v>
       </c>
@@ -570,4 +593,118 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BBE6FAD-B133-4AAC-8B1A-CD98E49FFFDA}">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4">
+        <v>5234</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1" s="4">
+        <v>1</v>
+      </c>
+      <c r="J1" s="7">
+        <v>45467</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="9">
+        <v>21.33</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="10">
+        <v>0</v>
+      </c>
+      <c r="I2" s="10">
+        <v>0</v>
+      </c>
+      <c r="J2" s="7">
+        <v>45477</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="10">
+        <v>970</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="10">
+        <v>0</v>
+      </c>
+      <c r="I3" s="10">
+        <v>1</v>
+      </c>
+      <c r="J3" s="7">
+        <v>45422</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Commission task completed, testing done. Left full test with real data
</commit_message>
<xml_diff>
--- a/NBSForm.xlsx
+++ b/NBSForm.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\winnie\Desktop\code playground\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Han Ming\Documents\Han Ming\python learning\IFAST-automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D30BCC79-FB01-4480-9B66-54E41105AC1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B623C2-3F19-4702-9D4E-CF233F094DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
   <si>
     <t>Acc No.</t>
   </si>
@@ -68,9 +68,6 @@
     <t>Purdy, Tim</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>1- Yes</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>Brown, Jarrad</t>
+  </si>
+  <si>
+    <t>P0519961</t>
   </si>
 </sst>
 </file>
@@ -498,23 +498,23 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -543,18 +543,18 @@
         <v>8</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B2" s="10">
         <v>13</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>11</v>
@@ -566,7 +566,7 @@
         <v>13</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H2" s="10">
         <v>0</v>
@@ -578,15 +578,15 @@
         <v>45337</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N5" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N5" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -597,18 +597,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BBE6FAD-B133-4AAC-8B1A-CD98E49FFFDA}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -640,15 +640,15 @@
         <v>45467</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="9">
         <v>21.33</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>11</v>
@@ -660,7 +660,7 @@
         <v>13</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H2" s="10">
         <v>0</v>
@@ -672,15 +672,15 @@
         <v>45477</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="10">
         <v>970</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>11</v>
@@ -692,7 +692,7 @@
         <v>13</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H3" s="10">
         <v>0</v>
@@ -702,6 +702,38 @@
       </c>
       <c r="J3" s="7">
         <v>45422</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="10">
+        <v>13</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="10">
+        <v>0</v>
+      </c>
+      <c r="I4" s="10">
+        <v>1</v>
+      </c>
+      <c r="J4" s="7">
+        <v>45337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
error handling, file cleanup
</commit_message>
<xml_diff>
--- a/NBSForm.xlsx
+++ b/NBSForm.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Han Ming\Documents\Han Ming\python learning\IFAST-automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Han Ming\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B623C2-3F19-4702-9D4E-CF233F094DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6172935B-C850-465C-AE8F-778610E48C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="25">
   <si>
     <t>Acc No.</t>
   </si>
@@ -547,14 +547,14 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="10">
-        <v>13</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>19</v>
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="4">
+        <v>5234</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>11</v>
@@ -565,28 +565,119 @@
       <c r="F2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0</v>
+      </c>
+      <c r="I2" s="4">
+        <v>1</v>
+      </c>
+      <c r="J2" s="7">
+        <v>45467</v>
+      </c>
+      <c r="N2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="9">
+        <v>21.33</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="10">
+        <v>0</v>
+      </c>
+      <c r="I3" s="10">
+        <v>0</v>
+      </c>
+      <c r="J3" s="7">
+        <v>45477</v>
+      </c>
+      <c r="N3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="10">
+        <v>970</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="10">
-        <v>0</v>
-      </c>
-      <c r="I2" s="10">
+      <c r="H4" s="10">
+        <v>0</v>
+      </c>
+      <c r="I4" s="10">
         <v>1</v>
       </c>
-      <c r="J2" s="7">
+      <c r="J4" s="7">
+        <v>45422</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="10">
+        <v>13</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="10">
+        <v>0</v>
+      </c>
+      <c r="I5" s="10">
+        <v>1</v>
+      </c>
+      <c r="J5" s="7">
         <v>45337</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="N4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="N5" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -600,7 +691,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="J4" sqref="A1:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
dynamic file path, compiled into .exe file
</commit_message>
<xml_diff>
--- a/NBSForm.xlsx
+++ b/NBSForm.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Han Ming\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Han Ming\Documents\Han Ming\python learning\IFAST-automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6172935B-C850-465C-AE8F-778610E48C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9295FA0F-B7B4-420F-88D9-124243F4B07D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="36">
   <si>
     <t>Acc No.</t>
   </si>
@@ -68,9 +68,6 @@
     <t>Purdy, Tim</t>
   </si>
   <si>
-    <t>1- Yes</t>
-  </si>
-  <si>
     <t>0 - No</t>
   </si>
   <si>
@@ -96,13 +93,49 @@
   </si>
   <si>
     <t>P0519961</t>
+  </si>
+  <si>
+    <t>For FAF's</t>
+  </si>
+  <si>
+    <t>1 - Yes</t>
+  </si>
+  <si>
+    <t>Agent name to follow exactly as in BBO</t>
+  </si>
+  <si>
+    <t>lastname, firstname</t>
+  </si>
+  <si>
+    <t>Provider to follow exactly as in BBO</t>
+  </si>
+  <si>
+    <t>Product to follow exactly as in BBO</t>
+  </si>
+  <si>
+    <t>Program will only read in Sheet1</t>
+  </si>
+  <si>
+    <t>Accounts that are new should not be inside the excel sheet (does not have a single row at all)</t>
+  </si>
+  <si>
+    <t>When program first starts, command prompt will ask user to sign up first</t>
+  </si>
+  <si>
+    <t>Once signed up, press enter on command prompt to run the program</t>
+  </si>
+  <si>
+    <t>*Must put NBSForm.xlsx in Desktop folder, make sure to save file before running</t>
+  </si>
+  <si>
+    <t>The program can run in the background, not needed to tab to the window itself</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,13 +164,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -156,10 +201,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -187,8 +233,15 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -492,10 +545,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -512,9 +565,11 @@
     <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
     <col min="12" max="14" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="41.33203125" customWidth="1"/>
+    <col min="16" max="16" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -543,53 +598,70 @@
         <v>8</v>
       </c>
       <c r="J1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="11"/>
+    </row>
+    <row r="2" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="4">
-        <v>5234</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="B2" s="9">
+        <v>21.33</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="4">
+        <v>19</v>
+      </c>
+      <c r="H2" s="10">
         <v>0</v>
       </c>
-      <c r="I2" s="4">
-        <v>1</v>
+      <c r="I2" s="10">
+        <v>0</v>
       </c>
       <c r="J2" s="7">
-        <v>45467</v>
-      </c>
-      <c r="N2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>45477</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" s="11"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="9">
-        <v>21.33</v>
+        <v>20</v>
+      </c>
+      <c r="B3" s="10">
+        <v>970</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>11</v>
@@ -600,87 +672,130 @@
       <c r="F3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>20</v>
+      <c r="G3" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="H3" s="10">
         <v>0</v>
       </c>
       <c r="I3" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" s="7">
-        <v>45477</v>
-      </c>
-      <c r="N3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="10">
-        <v>970</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="10">
-        <v>0</v>
-      </c>
-      <c r="I4" s="10">
-        <v>1</v>
-      </c>
-      <c r="J4" s="7">
         <v>45422</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="10">
-        <v>13</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="10">
-        <v>0</v>
-      </c>
-      <c r="I5" s="10">
-        <v>1</v>
-      </c>
-      <c r="J5" s="7">
-        <v>45337</v>
-      </c>
+      <c r="N3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="8"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="7"/>
+      <c r="N4" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="O4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="M6" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N7" s="11"/>
+      <c r="O7" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N8" s="11"/>
+      <c r="O8" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N10" s="11"/>
+      <c r="O10" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N11" s="11"/>
+      <c r="O11" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N12" s="11"/>
+      <c r="O12" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="M6:Q6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -733,13 +848,13 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="9">
         <v>21.33</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>11</v>
@@ -751,7 +866,7 @@
         <v>13</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H2" s="10">
         <v>0</v>
@@ -765,13 +880,13 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="10">
         <v>970</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>11</v>
@@ -783,7 +898,7 @@
         <v>13</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H3" s="10">
         <v>0</v>
@@ -797,13 +912,13 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="10">
         <v>13</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>11</v>
@@ -815,7 +930,7 @@
         <v>13</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H4" s="10">
         <v>0</v>

</xml_diff>